<commit_message>
Merged PR 11742: Fix data source file update - merge with asnull option selected and partial field set
Fix data source file update - merge with asnull option selected and partial field set

Related work items: #64805
</commit_message>
<xml_diff>
--- a/CalculateFunding.Services.Datasets.UnitTests/TestItems/PE_and_Sports_Grant_Data_AsNull_result.xlsx
+++ b/CalculateFunding.Services.Datasets.UnitTests/TestItems/PE_and_Sports_Grant_Data_AsNull_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\sinem\CalculateFunding-Backend\CalculateFunding.Services.Datasets.UnitTests\TestItems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5866F972-8EA5-4101-8326-252DF47FB2CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54CCCC7-E81B-41BF-A899-A0E6F16AC805}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="5380" windowWidth="28800" windowHeight="15290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PE and Sport Grant" sheetId="1" r:id="rId1"/>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1282,7 +1282,7 @@
         <v>0</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -7196,9 +7196,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7411,27 +7414,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA5BD8A6-8524-4FB3-BADC-0E49138F02CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{893FC4BE-952F-4B77-A17C-02E1E16AD86B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7e3e27cc-3a1c-477d-aac6-02b314d79f5e"/>
-    <ds:schemaRef ds:uri="ab119141-cd66-4087-86bb-8e659032e627"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7456,9 +7447,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{893FC4BE-952F-4B77-A17C-02E1E16AD86B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA5BD8A6-8524-4FB3-BADC-0E49138F02CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7e3e27cc-3a1c-477d-aac6-02b314d79f5e"/>
+    <ds:schemaRef ds:uri="ab119141-cd66-4087-86bb-8e659032e627"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>